<commit_message>
Added (almost) full support for auto filters, missing custom date filters.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Ranges/SortExample.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Ranges/SortExample.xlsx
@@ -45,7 +45,7 @@
     <x:t>a</x:t>
   </x:si>
   <x:si>
-    <x:t>.Sort(XLSortOrientation.LeftToRight) = Sort Range Left to Right, Ascendingly, Ignore Blanks, Ignore Case</x:t>
+    <x:t>.SortLeftToRight() = Sort Range Left to Right, Ascendingly, Ignore Blanks, Ignore Case</x:t>
   </x:si>
   <x:si>
     <x:t>.SortColumns.Add(1, XLSortOrder.Ascending, false, true) = Sort Col 1 Asc, Match Blanks, Match Case</x:t>
@@ -57,7 +57,7 @@
     <x:t>.Sort() = Sort range using the parameters defined in SortColumns</x:t>
   </x:si>
   <x:si>
-    <x:t>.Sort("2, 1 DESC", true) = Sort Range Top to Bottom, Col 2 Asc, Col 1 Desc, Ignore Blanks, Match Case</x:t>
+    <x:t>.Sort("2, 1 DESC", XLSortOrder.Ascending, true) = Sort Range Top to Bottom, Col 2 Asc, Col 1 Desc, Ignore Blanks, Match Case</x:t>
   </x:si>
   <x:si>
     <x:t>.Sort(XLSortOrder.Descending, true) = Sort Range Top to Bottom, Descendingly, Ignore Blanks, Match Case</x:t>
@@ -746,7 +746,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:H10"/>
+  <x:dimension ref="A1:H15"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
@@ -897,6 +897,26 @@
       <x:c r="H10" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
+    </x:row>
+    <x:row r="11" spans="1:8">
+      <x:c r="A11" s="0" t="s"/>
+      <x:c r="D11" s="0" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:8">
+      <x:c r="A12" s="0" t="s"/>
+      <x:c r="D12" s="0" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:8">
+      <x:c r="A13" s="0" t="s"/>
+      <x:c r="D13" s="0" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:8">
+      <x:c r="A14" s="0" t="s"/>
+      <x:c r="D14" s="0" t="s"/>
+    </x:row>
+    <x:row r="15" spans="1:8">
+      <x:c r="A15" s="0" t="s"/>
+      <x:c r="D15" s="0" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Fixed issue when sorting ranges with blank cells.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Ranges/SortExample.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Ranges/SortExample.xlsx
@@ -583,6 +583,8 @@
       <x:c r="C3" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="D3" s="0" t="s"/>
+      <x:c r="E3" s="0" t="s"/>
       <x:c r="F3" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
@@ -601,6 +603,8 @@
       <x:c r="C4" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D4" s="0" t="s"/>
+      <x:c r="E4" s="0" t="s"/>
       <x:c r="F4" s="3" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -619,6 +623,8 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C5" s="4" t="s"/>
+      <x:c r="D5" s="0" t="s"/>
+      <x:c r="E5" s="0" t="s"/>
       <x:c r="F5" s="5" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -639,6 +645,8 @@
       <x:c r="C6" s="6" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D6" s="0" t="s"/>
+      <x:c r="E6" s="0" t="s"/>
       <x:c r="F6" s="7" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -659,6 +667,8 @@
       <x:c r="C7" s="5" t="s">
         <x:v>7</x:v>
       </x:c>
+      <x:c r="D7" s="0" t="s"/>
+      <x:c r="E7" s="0" t="s"/>
       <x:c r="F7" s="8" t="s"/>
       <x:c r="G7" s="8" t="s">
         <x:v>7</x:v>
@@ -675,6 +685,8 @@
       <x:c r="C8" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D8" s="0" t="s"/>
+      <x:c r="E8" s="0" t="s"/>
       <x:c r="F8" s="4" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -693,6 +705,8 @@
       <x:c r="C9" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
+      <x:c r="D9" s="0" t="s"/>
+      <x:c r="E9" s="0" t="s"/>
       <x:c r="F9" s="9" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -711,6 +725,8 @@
       <x:c r="C10" s="7" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D10" s="0" t="s"/>
+      <x:c r="E10" s="0" t="s"/>
       <x:c r="F10" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -979,6 +995,8 @@
       <x:c r="C5" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D5" s="0" t="s"/>
+      <x:c r="E5" s="0" t="s"/>
       <x:c r="F5" s="8" t="s"/>
       <x:c r="G5" s="8" t="s">
         <x:v>7</x:v>
@@ -995,6 +1013,8 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C6" s="4" t="s"/>
+      <x:c r="D6" s="0" t="s"/>
+      <x:c r="E6" s="0" t="s"/>
       <x:c r="F6" s="7" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -1015,6 +1035,8 @@
       <x:c r="C7" s="6" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D7" s="0" t="s"/>
+      <x:c r="E7" s="0" t="s"/>
       <x:c r="F7" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -1035,6 +1057,8 @@
       <x:c r="C8" s="5" t="s">
         <x:v>7</x:v>
       </x:c>
+      <x:c r="D8" s="0" t="s"/>
+      <x:c r="E8" s="0" t="s"/>
       <x:c r="F8" s="3" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1053,6 +1077,8 @@
       <x:c r="C9" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D9" s="0" t="s"/>
+      <x:c r="E9" s="0" t="s"/>
       <x:c r="F9" s="5" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1073,6 +1099,8 @@
       <x:c r="C10" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
+      <x:c r="D10" s="0" t="s"/>
+      <x:c r="E10" s="0" t="s"/>
       <x:c r="F10" s="4" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1091,6 +1119,8 @@
       <x:c r="C11" s="7" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D11" s="0" t="s"/>
+      <x:c r="E11" s="0" t="s"/>
       <x:c r="F11" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1107,6 +1137,8 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C12" s="9" t="s"/>
+      <x:c r="D12" s="0" t="s"/>
+      <x:c r="E12" s="0" t="s"/>
       <x:c r="F12" s="9" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1155,6 +1187,8 @@
       <x:c r="C3" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D3" s="0" t="s"/>
+      <x:c r="E3" s="0" t="s"/>
       <x:c r="F3" s="9" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1171,6 +1205,8 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C4" s="4" t="s"/>
+      <x:c r="D4" s="0" t="s"/>
+      <x:c r="E4" s="0" t="s"/>
       <x:c r="F4" s="4" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1189,6 +1225,8 @@
       <x:c r="C5" s="6" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D5" s="0" t="s"/>
+      <x:c r="E5" s="0" t="s"/>
       <x:c r="F5" s="7" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -1209,6 +1247,8 @@
       <x:c r="C6" s="5" t="s">
         <x:v>7</x:v>
       </x:c>
+      <x:c r="D6" s="0" t="s"/>
+      <x:c r="E6" s="0" t="s"/>
       <x:c r="F6" s="8" t="s"/>
       <x:c r="G6" s="8" t="s">
         <x:v>7</x:v>
@@ -1225,6 +1265,8 @@
       <x:c r="C7" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D7" s="0" t="s"/>
+      <x:c r="E7" s="0" t="s"/>
       <x:c r="F7" s="5" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1245,6 +1287,8 @@
       <x:c r="C8" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
+      <x:c r="D8" s="0" t="s"/>
+      <x:c r="E8" s="0" t="s"/>
       <x:c r="F8" s="3" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1265,6 +1309,8 @@
       <x:c r="C9" s="7" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D9" s="0" t="s"/>
+      <x:c r="E9" s="0" t="s"/>
       <x:c r="F9" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -1283,6 +1329,8 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C10" s="9" t="s"/>
+      <x:c r="D10" s="0" t="s"/>
+      <x:c r="E10" s="0" t="s"/>
       <x:c r="F10" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1327,6 +1375,8 @@
       <x:c r="A3" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="B3" s="0" t="s"/>
+      <x:c r="C3" s="0" t="s"/>
       <x:c r="D3" s="9" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -1335,6 +1385,8 @@
       <x:c r="A4" s="4" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="B4" s="0" t="s"/>
+      <x:c r="C4" s="0" t="s"/>
       <x:c r="D4" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1343,18 +1395,24 @@
       <x:c r="A5" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
+      <x:c r="B5" s="0" t="s"/>
+      <x:c r="C5" s="0" t="s"/>
       <x:c r="D5" s="7" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
       <x:c r="A6" s="5" t="s"/>
+      <x:c r="B6" s="0" t="s"/>
+      <x:c r="C6" s="0" t="s"/>
       <x:c r="D6" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
       <x:c r="A7" s="8" t="s"/>
+      <x:c r="B7" s="0" t="s"/>
+      <x:c r="C7" s="0" t="s"/>
       <x:c r="D7" s="4" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1363,6 +1421,8 @@
       <x:c r="A8" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
+      <x:c r="B8" s="0" t="s"/>
+      <x:c r="C8" s="0" t="s"/>
       <x:c r="D8" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -1371,12 +1431,16 @@
       <x:c r="A9" s="7" t="s">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="B9" s="0" t="s"/>
+      <x:c r="C9" s="0" t="s"/>
       <x:c r="D9" s="8" t="s"/>
     </x:row>
     <x:row r="10" spans="1:4">
       <x:c r="A10" s="9" t="s">
         <x:v>14</x:v>
       </x:c>
+      <x:c r="B10" s="0" t="s"/>
+      <x:c r="C10" s="0" t="s"/>
       <x:c r="D10" s="5" t="s"/>
     </x:row>
   </x:sheetData>
@@ -1419,6 +1483,8 @@
       <x:c r="C3" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D3" s="0" t="s"/>
+      <x:c r="E3" s="0" t="s"/>
       <x:c r="F3" s="7" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -1437,6 +1503,8 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C4" s="4" t="s"/>
+      <x:c r="D4" s="0" t="s"/>
+      <x:c r="E4" s="0" t="s"/>
       <x:c r="F4" s="5" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1457,6 +1525,8 @@
       <x:c r="C5" s="6" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D5" s="0" t="s"/>
+      <x:c r="E5" s="0" t="s"/>
       <x:c r="F5" s="3" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1477,6 +1547,8 @@
       <x:c r="C6" s="5" t="s">
         <x:v>7</x:v>
       </x:c>
+      <x:c r="D6" s="0" t="s"/>
+      <x:c r="E6" s="0" t="s"/>
       <x:c r="F6" s="4" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1493,6 +1565,8 @@
       <x:c r="C7" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D7" s="0" t="s"/>
+      <x:c r="E7" s="0" t="s"/>
       <x:c r="F7" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -1513,6 +1587,8 @@
       <x:c r="C8" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
+      <x:c r="D8" s="0" t="s"/>
+      <x:c r="E8" s="0" t="s"/>
       <x:c r="F8" s="9" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1531,6 +1607,8 @@
       <x:c r="C9" s="7" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D9" s="0" t="s"/>
+      <x:c r="E9" s="0" t="s"/>
       <x:c r="F9" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1547,6 +1625,8 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C10" s="9" t="s"/>
+      <x:c r="D10" s="0" t="s"/>
+      <x:c r="E10" s="0" t="s"/>
       <x:c r="F10" s="8" t="s"/>
       <x:c r="G10" s="8" t="s">
         <x:v>7</x:v>

</xml_diff>

<commit_message>
Improved performance of previous fix.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Ranges/SortExample.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Ranges/SortExample.xlsx
@@ -583,8 +583,6 @@
       <x:c r="C3" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s"/>
-      <x:c r="E3" s="0" t="s"/>
       <x:c r="F3" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
@@ -603,8 +601,6 @@
       <x:c r="C4" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D4" s="0" t="s"/>
-      <x:c r="E4" s="0" t="s"/>
       <x:c r="F4" s="3" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -623,8 +619,6 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C5" s="4" t="s"/>
-      <x:c r="D5" s="0" t="s"/>
-      <x:c r="E5" s="0" t="s"/>
       <x:c r="F5" s="5" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -645,8 +639,6 @@
       <x:c r="C6" s="6" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D6" s="0" t="s"/>
-      <x:c r="E6" s="0" t="s"/>
       <x:c r="F6" s="7" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -667,8 +659,6 @@
       <x:c r="C7" s="5" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D7" s="0" t="s"/>
-      <x:c r="E7" s="0" t="s"/>
       <x:c r="F7" s="8" t="s"/>
       <x:c r="G7" s="8" t="s">
         <x:v>7</x:v>
@@ -685,8 +675,6 @@
       <x:c r="C8" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D8" s="0" t="s"/>
-      <x:c r="E8" s="0" t="s"/>
       <x:c r="F8" s="4" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -705,8 +693,6 @@
       <x:c r="C9" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D9" s="0" t="s"/>
-      <x:c r="E9" s="0" t="s"/>
       <x:c r="F9" s="9" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -725,8 +711,6 @@
       <x:c r="C10" s="7" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D10" s="0" t="s"/>
-      <x:c r="E10" s="0" t="s"/>
       <x:c r="F10" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -995,8 +979,6 @@
       <x:c r="C5" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D5" s="0" t="s"/>
-      <x:c r="E5" s="0" t="s"/>
       <x:c r="F5" s="8" t="s"/>
       <x:c r="G5" s="8" t="s">
         <x:v>7</x:v>
@@ -1013,8 +995,6 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C6" s="4" t="s"/>
-      <x:c r="D6" s="0" t="s"/>
-      <x:c r="E6" s="0" t="s"/>
       <x:c r="F6" s="7" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -1035,8 +1015,6 @@
       <x:c r="C7" s="6" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D7" s="0" t="s"/>
-      <x:c r="E7" s="0" t="s"/>
       <x:c r="F7" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -1057,8 +1035,6 @@
       <x:c r="C8" s="5" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D8" s="0" t="s"/>
-      <x:c r="E8" s="0" t="s"/>
       <x:c r="F8" s="3" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1077,8 +1053,6 @@
       <x:c r="C9" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D9" s="0" t="s"/>
-      <x:c r="E9" s="0" t="s"/>
       <x:c r="F9" s="5" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1099,8 +1073,6 @@
       <x:c r="C10" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D10" s="0" t="s"/>
-      <x:c r="E10" s="0" t="s"/>
       <x:c r="F10" s="4" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1119,8 +1091,6 @@
       <x:c r="C11" s="7" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D11" s="0" t="s"/>
-      <x:c r="E11" s="0" t="s"/>
       <x:c r="F11" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1137,8 +1107,6 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C12" s="9" t="s"/>
-      <x:c r="D12" s="0" t="s"/>
-      <x:c r="E12" s="0" t="s"/>
       <x:c r="F12" s="9" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1187,8 +1155,6 @@
       <x:c r="C3" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s"/>
-      <x:c r="E3" s="0" t="s"/>
       <x:c r="F3" s="9" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1205,8 +1171,6 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C4" s="4" t="s"/>
-      <x:c r="D4" s="0" t="s"/>
-      <x:c r="E4" s="0" t="s"/>
       <x:c r="F4" s="4" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1225,8 +1189,6 @@
       <x:c r="C5" s="6" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D5" s="0" t="s"/>
-      <x:c r="E5" s="0" t="s"/>
       <x:c r="F5" s="7" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -1247,8 +1209,6 @@
       <x:c r="C6" s="5" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D6" s="0" t="s"/>
-      <x:c r="E6" s="0" t="s"/>
       <x:c r="F6" s="8" t="s"/>
       <x:c r="G6" s="8" t="s">
         <x:v>7</x:v>
@@ -1265,8 +1225,6 @@
       <x:c r="C7" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D7" s="0" t="s"/>
-      <x:c r="E7" s="0" t="s"/>
       <x:c r="F7" s="5" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1287,8 +1245,6 @@
       <x:c r="C8" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D8" s="0" t="s"/>
-      <x:c r="E8" s="0" t="s"/>
       <x:c r="F8" s="3" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1309,8 +1265,6 @@
       <x:c r="C9" s="7" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D9" s="0" t="s"/>
-      <x:c r="E9" s="0" t="s"/>
       <x:c r="F9" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -1329,8 +1283,6 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C10" s="9" t="s"/>
-      <x:c r="D10" s="0" t="s"/>
-      <x:c r="E10" s="0" t="s"/>
       <x:c r="F10" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1375,8 +1327,6 @@
       <x:c r="A3" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s"/>
-      <x:c r="C3" s="0" t="s"/>
       <x:c r="D3" s="9" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -1385,8 +1335,6 @@
       <x:c r="A4" s="4" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s"/>
-      <x:c r="C4" s="0" t="s"/>
       <x:c r="D4" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1395,24 +1343,18 @@
       <x:c r="A5" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="B5" s="0" t="s"/>
-      <x:c r="C5" s="0" t="s"/>
       <x:c r="D5" s="7" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
       <x:c r="A6" s="5" t="s"/>
-      <x:c r="B6" s="0" t="s"/>
-      <x:c r="C6" s="0" t="s"/>
       <x:c r="D6" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
       <x:c r="A7" s="8" t="s"/>
-      <x:c r="B7" s="0" t="s"/>
-      <x:c r="C7" s="0" t="s"/>
       <x:c r="D7" s="4" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1421,8 +1363,6 @@
       <x:c r="A8" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="B8" s="0" t="s"/>
-      <x:c r="C8" s="0" t="s"/>
       <x:c r="D8" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -1431,16 +1371,12 @@
       <x:c r="A9" s="7" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="B9" s="0" t="s"/>
-      <x:c r="C9" s="0" t="s"/>
       <x:c r="D9" s="8" t="s"/>
     </x:row>
     <x:row r="10" spans="1:4">
       <x:c r="A10" s="9" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="B10" s="0" t="s"/>
-      <x:c r="C10" s="0" t="s"/>
       <x:c r="D10" s="5" t="s"/>
     </x:row>
   </x:sheetData>
@@ -1483,8 +1419,6 @@
       <x:c r="C3" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s"/>
-      <x:c r="E3" s="0" t="s"/>
       <x:c r="F3" s="7" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -1503,8 +1437,6 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C4" s="4" t="s"/>
-      <x:c r="D4" s="0" t="s"/>
-      <x:c r="E4" s="0" t="s"/>
       <x:c r="F4" s="5" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1525,8 +1457,6 @@
       <x:c r="C5" s="6" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D5" s="0" t="s"/>
-      <x:c r="E5" s="0" t="s"/>
       <x:c r="F5" s="3" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1547,8 +1477,6 @@
       <x:c r="C6" s="5" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D6" s="0" t="s"/>
-      <x:c r="E6" s="0" t="s"/>
       <x:c r="F6" s="4" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1565,8 +1493,6 @@
       <x:c r="C7" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D7" s="0" t="s"/>
-      <x:c r="E7" s="0" t="s"/>
       <x:c r="F7" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -1587,8 +1513,6 @@
       <x:c r="C8" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D8" s="0" t="s"/>
-      <x:c r="E8" s="0" t="s"/>
       <x:c r="F8" s="9" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1607,8 +1531,6 @@
       <x:c r="C9" s="7" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D9" s="0" t="s"/>
-      <x:c r="E9" s="0" t="s"/>
       <x:c r="F9" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1625,8 +1547,6 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C10" s="9" t="s"/>
-      <x:c r="D10" s="0" t="s"/>
-      <x:c r="E10" s="0" t="s"/>
       <x:c r="F10" s="8" t="s"/>
       <x:c r="G10" s="8" t="s">
         <x:v>7</x:v>

</xml_diff>